<commit_message>
3.0.9: Implement ignoredProperty option to field.
</commit_message>
<xml_diff>
--- a/meta/objects2/BlancoValueObjectSuperClass.xlsx
+++ b/meta/objects2/BlancoValueObjectSuperClass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799D6418-CD14-B842-93AA-0E6AEE5F36D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043FE837-4803-E543-AAA3-15C5CC902646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="2960" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>クラス名</t>
   </si>
@@ -285,6 +285,32 @@
   </si>
   <si>
     <t>引数２</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ヒキスウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>kotlinでは無視</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ignoredField</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>無視されます</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ムシ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>stringField4</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>引数4</t>
     <rPh sb="0" eb="1">
       <t xml:space="preserve">ヒキスウ </t>
     </rPh>
@@ -840,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -935,6 +961,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -964,22 +1003,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,10 +1414,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1405,33 +1428,33 @@
     <col min="6" max="6" width="18.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
     <col min="8" max="13" width="8.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="28" style="1" customWidth="1"/>
-    <col min="18" max="18" width="33.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="1"/>
+    <col min="14" max="15" width="8.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="28" style="1" customWidth="1"/>
+    <col min="19" max="19" width="33.33203125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19">
+    <row r="1" spans="1:18" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +1463,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1475,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="45"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1464,7 +1487,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="45"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1476,7 +1499,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="45"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1488,7 +1511,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="45"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" s="36" t="s">
         <v>27</v>
       </c>
@@ -1509,8 +1532,9 @@
       <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="36" t="s">
         <v>37</v>
       </c>
@@ -1529,8 +1553,9 @@
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="36" t="s">
         <v>22</v>
       </c>
@@ -1551,8 +1576,9 @@
       <c r="N12"/>
       <c r="O12"/>
       <c r="P12"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="36" t="s">
         <v>24</v>
       </c>
@@ -1573,11 +1599,12 @@
       <c r="N13"/>
       <c r="O13"/>
       <c r="P13"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
@@ -1591,8 +1618,9 @@
       <c r="N14"/>
       <c r="O14"/>
       <c r="P14"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1609,8 +1637,9 @@
       <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="28" t="s">
         <v>18</v>
       </c>
@@ -1620,7 +1649,7 @@
       <c r="E16" s="30"/>
       <c r="F16" s="46"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:19">
       <c r="A17" s="31" t="s">
         <v>0</v>
       </c>
@@ -1638,14 +1667,15 @@
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
+      <c r="P17" s="48"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="48"/>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
       <c r="I18" s="48"/>
@@ -1655,8 +1685,9 @@
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
       <c r="O18" s="48"/>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="P18" s="48"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1673,8 +1704,9 @@
       <c r="N19"/>
       <c r="O19"/>
       <c r="P19"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1694,79 +1726,84 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A21" s="51" t="s">
+      <c r="R20" s="12"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" ht="13.5" customHeight="1">
+      <c r="A21" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="50" t="s">
+      <c r="F21" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="52" t="s">
+      <c r="G21" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="58" t="s">
+      <c r="I21" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="56" t="s">
+      <c r="J21" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="56" t="s">
+      <c r="K21" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="56" t="s">
+      <c r="L21" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="56" t="s">
+      <c r="M21" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="56" t="s">
+      <c r="N21" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="50" t="s">
+      <c r="O21" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="P21" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="14"/>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="27"/>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="Q21" s="55"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="14"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="56"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="27"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="16">
         <v>1</v>
       </c>
@@ -1795,14 +1832,15 @@
       <c r="N23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="18" t="s">
+      <c r="O23" s="18"/>
+      <c r="P23" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
-      <c r="R23" s="26"/>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="R23" s="19"/>
+      <c r="S23" s="26"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="16">
         <v>2</v>
       </c>
@@ -1831,20 +1869,31 @@
       <c r="N24" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O24" s="18"/>
+      <c r="P24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
-      <c r="R24" s="20"/>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="20"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="16">
+        <v>3</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="E25" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
@@ -1853,32 +1902,52 @@
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="19"/>
+      <c r="O25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="20"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="16">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="E26" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="L26" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
-      <c r="P26" s="19"/>
+      <c r="P26" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="Q26" s="19"/>
-      <c r="R26" s="20"/>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="R26" s="19"/>
+      <c r="S26" s="20"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="21"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23"/>
@@ -1894,13 +1963,14 @@
       <c r="M27" s="23"/>
       <c r="N27" s="23"/>
       <c r="O27" s="23"/>
-      <c r="P27" s="24"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="24"/>
-      <c r="R27" s="25"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="O21:P22"/>
+  <mergeCells count="16">
+    <mergeCell ref="P21:Q22"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
@@ -1909,16 +1979,17 @@
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
-    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E43:N43" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E43:O43" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1931,7 +2002,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{7083602A-A73F-BE48-A359-8D659B03A9B3}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:N27" xr:uid="{DC9EBF38-7703-0D4E-BA7E-C817D1AB0B2C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:O27" xr:uid="{DC9EBF38-7703-0D4E-BA7E-C817D1AB0B2C}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>